<commit_message>
PLU activation function added
</commit_message>
<xml_diff>
--- a/ActivationFunctions/Sigmoid.xlsx
+++ b/ActivationFunctions/Sigmoid.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\NeuralNetwork\ActivationFunctions\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6671582-A87A-47AC-8D66-5ACC24344C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,9 +28,13 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,25 +83,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -372,53 +358,40 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D5EB-48BF-B251-7B5A87969450}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="45177472"/>
-        <c:axId val="45175552"/>
+        <c:dLbls/>
+        <c:axId val="109936640"/>
+        <c:axId val="109938176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45177472"/>
+        <c:axId val="109936640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45175552"/>
+        <c:crossAx val="109938176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45175552"/>
+        <c:axId val="109938176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45177472"/>
+        <c:crossAx val="109936640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.25"/>
@@ -426,36 +399,25 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -484,12 +446,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -782,29 +742,21 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E976-40DA-A889-B1474854642F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="830915184"/>
-        <c:axId val="735897312"/>
+        <c:dLbls/>
+        <c:axId val="122810368"/>
+        <c:axId val="122811904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="830915184"/>
+        <c:axId val="122810368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -822,7 +774,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -857,16 +808,15 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="735897312"/>
+        <c:crossAx val="122811904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="735897312"/>
+        <c:axId val="122811904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -884,7 +834,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -919,7 +868,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="830915184"/>
+        <c:crossAx val="122810368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -933,14 +882,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -969,7 +917,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1551,7 +1499,7 @@
         <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1587,7 +1535,7 @@
         <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA32D702-2265-5F56-A7D0-6E69599400F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DA32D702-2265-5F56-A7D0-6E69599400F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1609,9 +1557,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1649,7 +1597,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1683,7 +1631,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1718,10 +1665,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1894,16 +1840,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>10</v>
       </c>
@@ -1919,7 +1865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>9.5</v>
       </c>
@@ -1932,7 +1878,7 @@
         <v>4.251956078844754E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1945,7 +1891,7 @@
         <v>5.4331148611126215E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>8.5</v>
       </c>
@@ -1958,7 +1904,7 @@
         <v>6.9329207188170436E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1971,7 +1917,7 @@
         <v>8.8313531066455536E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>7.5</v>
       </c>
@@ -1984,7 +1930,7 @@
         <v>1.1224705191021742E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1997,7 +1943,7 @@
         <v>1.4226511939867799E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6.5</v>
       </c>
@@ -2010,7 +1956,7 @@
         <v>1.7966795412664022E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2023,7 +1969,7 @@
         <v>2.2588329865455999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>5.5</v>
       </c>
@@ -2036,7 +1982,7 @@
         <v>2.8238122322437019E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>5</v>
       </c>
@@ -2049,7 +1995,7 @@
         <v>3.5051858272554033E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>4.5</v>
       </c>
@@ -2062,7 +2008,7 @@
         <v>4.3128972221281474E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2075,7 +2021,7 @@
         <v>5.2496792701753309E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>3.5</v>
       </c>
@@ -2088,7 +2034,7 @@
         <v>6.3064612593327574E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2101,7 +2047,7 @@
         <v>7.4573226035166432E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -2114,7 +2060,7 @@
         <v>8.6552393496248534E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2127,7 +2073,7 @@
         <v>9.8305966620740926E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>1.5</v>
       </c>
@@ -2140,7 +2086,7 @@
         <v>0.10894749688090702</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2153,7 +2099,7 @@
         <v>0.11750185610079725</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>0.5</v>
       </c>
@@ -2166,7 +2112,7 @@
         <v>0.12306704136879917</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2179,7 +2125,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>-0.5</v>
       </c>
@@ -2192,7 +2138,7 @@
         <v>0.12306704136879917</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>-1</v>
       </c>
@@ -2205,7 +2151,7 @@
         <v>0.11750185610079725</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>-1.5</v>
       </c>
@@ -2218,7 +2164,7 @@
         <v>0.10894749688090702</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>-2</v>
       </c>
@@ -2231,7 +2177,7 @@
         <v>9.8305966620740926E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>-2.5</v>
       </c>
@@ -2244,7 +2190,7 @@
         <v>8.6552393496248506E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>-3</v>
       </c>
@@ -2257,7 +2203,7 @@
         <v>7.4573226035166432E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>-3.5</v>
       </c>
@@ -2270,7 +2216,7 @@
         <v>6.3064612593327588E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>-4</v>
       </c>
@@ -2283,7 +2229,7 @@
         <v>5.2496792701753253E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>-4.5</v>
       </c>
@@ -2296,7 +2242,7 @@
         <v>4.3128972221281488E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -2309,7 +2255,7 @@
         <v>3.5051858272554075E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>-5.5</v>
       </c>
@@ -2322,7 +2268,7 @@
         <v>2.8238122322437029E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>-6</v>
       </c>
@@ -2335,7 +2281,7 @@
         <v>2.2588329865456069E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>-6.5</v>
       </c>
@@ -2348,7 +2294,7 @@
         <v>1.7966795412664063E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>-7</v>
       </c>
@@ -2361,7 +2307,7 @@
         <v>1.422651193986778E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>-7.5</v>
       </c>
@@ -2374,7 +2320,7 @@
         <v>1.1224705191021731E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>-8</v>
       </c>
@@ -2387,7 +2333,7 @@
         <v>8.8313531066455588E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>-8.5</v>
       </c>
@@ -2400,7 +2346,7 @@
         <v>6.9329207188169846E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>-9</v>
       </c>
@@ -2413,7 +2359,7 @@
         <v>5.4331148611126171E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>-9.5</v>
       </c>
@@ -2426,7 +2372,7 @@
         <v>4.2519560788447713E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>-10</v>
       </c>
@@ -2446,24 +2392,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sigmoid in combination with ReLu, LeReLu now possible, Batch processing with direct grad method. Draft only.
</commit_message>
<xml_diff>
--- a/ActivationFunctions/Sigmoid.xlsx
+++ b/ActivationFunctions/Sigmoid.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\NeuralNetwork\ActivationFunctions\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164D8DD1-B611-4541-8BB5-6114E4BF35C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,8 +29,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,25 +79,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -246,179 +228,166 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>0.99999999439720355</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9999999847700205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99999995860062441</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99999988746483792</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99999969409777301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99999916847197223</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99999773967570205</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99999385582539779</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99998329857815205</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99995460213129761</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99987660542401369</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99966464986953363</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9990889488055994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99752737684336534</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.99330714907571527</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99142251458628805</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.98901305736940681</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.9859363729567544</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="15">
                   <c:v>0.98201379003790845</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.97702263008997436</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.97068776924864364</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.96267311265587063</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
                   <c:v>0.95257412682243336</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.93991334982599239</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.92414181997875655</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.90465053510089055</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="17">
                   <c:v>0.88079707797788231</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.85195280196831058</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.81757447619364365</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.77729986117469108</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>0.7310585786300049</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.67917869917539297</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.62245933120185459</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.56217650088579807</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.5</c:v>
+                  <c:v>0.2689414213699951</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.43782349911420193</c:v>
+                  <c:v>0.11920292202211755</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.37754066879814541</c:v>
+                  <c:v>4.7425873177566781E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.32082130082460703</c:v>
+                  <c:v>1.7986209962091559E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.2689414213699951</c:v>
+                  <c:v>6.6928509242848554E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.22270013882530884</c:v>
+                  <c:v>2.4726231566347743E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.18242552380635635</c:v>
+                  <c:v>9.1105119440064539E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.14804719803168948</c:v>
+                  <c:v>3.3535013046647811E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.11920292202211755</c:v>
+                  <c:v>1.2339457598623172E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9.534946489910949E-2</c:v>
+                  <c:v>4.5397868702434395E-5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.5858180021243546E-2</c:v>
+                  <c:v>1.6701421848095181E-5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.0086650174007626E-2</c:v>
+                  <c:v>6.1441746022147182E-6</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.7425873177566781E-2</c:v>
+                  <c:v>2.2603242979035746E-6</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.7326887344129457E-2</c:v>
+                  <c:v>8.3152802766413209E-7</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.9312230751356319E-2</c:v>
+                  <c:v>3.0590222692562472E-7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.2977369910025615E-2</c:v>
+                  <c:v>1.1253516205509499E-7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.7986209962091559E-2</c:v>
+                  <c:v>4.1399375473943306E-8</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.4063627043245475E-2</c:v>
+                  <c:v>1.5229979512760349E-8</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.098694263059318E-2</c:v>
+                  <c:v>5.6027964061459406E-9</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.5774854137119841E-3</c:v>
+                  <c:v>2.0611536181902037E-9</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.6928509242848554E-3</c:v>
+                  <c:v>7.5825604221623851E-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D5EB-48BF-B251-7B5A87969450}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="109936640"/>
-        <c:axId val="109938176"/>
+        <c:dLbls/>
+        <c:axId val="129829120"/>
+        <c:axId val="129835008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109936640"/>
+        <c:axId val="129829120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109938176"/>
+        <c:crossAx val="129835008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109938176"/>
+        <c:axId val="129835008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109936640"/>
+        <c:crossAx val="129829120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.25"/>
@@ -426,36 +395,25 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -484,12 +442,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -656,155 +612,147 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>3.3240283353950166E-3</c:v>
+                  <c:v>1.1205592835239931E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.251956078844754E-3</c:v>
+                  <c:v>3.0459958535624582E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4331148611126215E-3</c:v>
+                  <c:v>8.2798747760845275E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9329207188170436E-3</c:v>
+                  <c:v>2.2507029882742626E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.8313531066455536E-3</c:v>
+                  <c:v>6.1180426683477429E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1224705191021742E-2</c:v>
+                  <c:v>1.6630546726564625E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4226511939867799E-2</c:v>
+                  <c:v>4.5206383777751979E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7966795412664022E-2</c:v>
+                  <c:v>1.2288273702651487E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2588329865455999E-2</c:v>
+                  <c:v>3.3402285820923139E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8238122322437019E-2</c:v>
+                  <c:v>9.079161547181531E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5051858272554033E-2</c:v>
+                  <c:v>2.4675869952986049E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.3128972221281474E-2</c:v>
+                  <c:v>6.704753415127363E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2496792701753309E-2</c:v>
+                  <c:v>1.8204423602435681E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.3064612593327574E-2</c:v>
+                  <c:v>4.9330185827198619E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.4573226035166432E-2</c:v>
+                  <c:v>1.3296113341580066E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.6552393496248534E-2</c:v>
+                  <c:v>3.5325412426582214E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.8305966620740926E-2</c:v>
+                  <c:v>9.0353319461823997E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.10894749688090702</c:v>
+                  <c:v>0.20998717080701323</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.11750185610079725</c:v>
+                  <c:v>0.3932238664829637</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12306704136879917</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.125</c:v>
+                  <c:v>0.3932238664829637</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.12306704136879917</c:v>
+                  <c:v>0.20998717080701301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.11750185610079725</c:v>
+                  <c:v>9.0353319461824275E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.10894749688090702</c:v>
+                  <c:v>3.5325412426582235E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.8305966620740926E-2</c:v>
+                  <c:v>1.3296113341580309E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.6552393496248506E-2</c:v>
+                  <c:v>4.9330185827200961E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.4573226035166432E-2</c:v>
+                  <c:v>1.8204423602436531E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.3064612593327588E-2</c:v>
+                  <c:v>6.7047534151294848E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.2496792701753253E-2</c:v>
+                  <c:v>2.4675869952969781E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.3128972221281488E-2</c:v>
+                  <c:v>9.0791615471903347E-5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.5051858272554075E-2</c:v>
+                  <c:v>3.3402285821206868E-5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.8238122322437029E-2</c:v>
+                  <c:v>1.2288273702666351E-5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.2588329865456069E-2</c:v>
+                  <c:v>4.5206383776752853E-6</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.7966795412664063E-2</c:v>
+                  <c:v>1.6630546724505427E-6</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.422651193986778E-2</c:v>
+                  <c:v>6.118042666989046E-7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.1224705191021731E-2</c:v>
+                  <c:v>2.2507029878186457E-7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.8313531066455588E-3</c:v>
+                  <c:v>8.2798747520070032E-8</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.9329207188169846E-3</c:v>
+                  <c:v>3.0459958561616146E-8</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.4331148611126171E-3</c:v>
+                  <c:v>1.1205592749509225E-8</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.2519560788447713E-3</c:v>
+                  <c:v>4.1223072278836992E-9</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.3240283353950773E-3</c:v>
+                  <c:v>1.5165120832825725E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E976-40DA-A889-B1474854642F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="122810368"/>
-        <c:axId val="122811904"/>
+        <c:dLbls/>
+        <c:axId val="131864832"/>
+        <c:axId val="131870720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122810368"/>
+        <c:axId val="131864832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -822,7 +770,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -857,16 +804,15 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122811904"/>
+        <c:crossAx val="131870720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122811904"/>
+        <c:axId val="131870720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -884,7 +830,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -919,7 +864,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122810368"/>
+        <c:crossAx val="131864832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -933,14 +878,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -969,7 +913,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -995,7 +939,7 @@
         <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1031,7 +975,7 @@
         <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA32D702-2265-5F56-A7D0-6E69599400F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DA32D702-2265-5F56-A7D0-6E69599400F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1053,9 +997,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1093,7 +1037,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1127,7 +1071,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1162,10 +1105,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1338,549 +1280,555 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B1" sqref="B1:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>10</v>
       </c>
       <c r="B1">
-        <f>(1/(1+EXP(-A1/$E$1)))</f>
-        <v>0.99330714907571527</v>
+        <f>(1/(1+EXP((-(A1+$E$2))/$E$1)))</f>
+        <v>0.99999999439720355</v>
       </c>
       <c r="C1">
-        <f xml:space="preserve"> (1/$E$1) * (1 / (1 + EXP(-A1 / $E$1)))*(1-(1 / (1 + EXP(-A1 / $E$1))))</f>
-        <v>3.3240283353950166E-3</v>
+        <f>(1/$E$1)*(1/(1+EXP((-A1-$E$2)/$E$1)))*(1-(1/(1+EXP((-A1-$E$2)/$E$1))))</f>
+        <v>1.1205592835239931E-8</v>
       </c>
       <c r="E1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>9.5</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B41" si="0">(1/(1+EXP(-A2/$E$1)))</f>
-        <v>0.99142251458628805</v>
+        <f t="shared" ref="B2:B41" si="0">(1/(1+EXP((-(A2+$E$2))/$E$1)))</f>
+        <v>0.9999999847700205</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C41" si="1" xml:space="preserve"> (1/$E$1) * (1 / (1 + EXP(-A2 / $E$1)))*(1-(1 / (1 + EXP(-A2 / $E$1))))</f>
-        <v>4.251956078844754E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C2:C41" si="1">(1/$E$1)*(1/(1+EXP((-A2-$E$2)/$E$1)))*(1-(1/(1+EXP((-A2-$E$2)/$E$1))))</f>
+        <v>3.0459958535624582E-8</v>
+      </c>
+      <c r="E2">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>9</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0.98901305736940681</v>
+        <v>0.99999995860062441</v>
       </c>
       <c r="C3">
         <f t="shared" si="1"/>
-        <v>5.4331148611126215E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8.2798747760845275E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>8.5</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>0.9859363729567544</v>
+        <v>0.99999988746483792</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>6.9329207188170436E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.2507029882742626E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>8</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0.98201379003790845</v>
+        <v>0.99999969409777301</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>8.8313531066455536E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6.1180426683477429E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>7.5</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.97702263008997436</v>
+        <v>0.99999916847197223</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>1.1224705191021742E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.6630546726564625E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.97068776924864364</v>
+        <v>0.99999773967570205</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>1.4226511939867799E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.5206383777751979E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6.5</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.96267311265587063</v>
+        <v>0.99999385582539779</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>1.7966795412664022E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.2288273702651487E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.95257412682243336</v>
+        <v>0.99998329857815205</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>2.2588329865455999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.3402285820923139E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>5.5</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.93991334982599239</v>
+        <v>0.99995460213129761</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>2.8238122322437019E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9.079161547181531E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0.92414181997875655</v>
+        <v>0.99987660542401369</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>3.5051858272554033E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.4675869952986049E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>4.5</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.90465053510089055</v>
+        <v>0.99966464986953363</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>4.3128972221281474E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6.704753415127363E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>0.88079707797788231</v>
+        <v>0.9990889488055994</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>5.2496792701753309E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.8204423602435681E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>3.5</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>0.85195280196831058</v>
+        <v>0.99752737684336534</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>6.3064612593327574E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.9330185827198619E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>0.81757447619364365</v>
+        <v>0.99330714907571527</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>7.4573226035166432E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.3296113341580066E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>2.5</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>0.77729986117469108</v>
+        <v>0.98201379003790845</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>8.6552393496248534E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.5325412426582214E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>0.7310585786300049</v>
+        <v>0.95257412682243336</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>9.8305966620740926E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9.0353319461823997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>1.5</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>0.67917869917539297</v>
+        <v>0.88079707797788231</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.10894749688090702</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.20998717080701323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>0.62245933120185459</v>
+        <v>0.7310585786300049</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>0.11750185610079725</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3932238664829637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>0.5</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>0.56217650088579807</v>
+        <v>0.5</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>0.12306704136879917</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>0</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.2689414213699951</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3932238664829637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>-0.5</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>0.43782349911420193</v>
+        <v>0.11920292202211755</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>0.12306704136879917</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.20998717080701301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>-1</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>0.37754066879814541</v>
+        <v>4.7425873177566781E-2</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>0.11750185610079725</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9.0353319461824275E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>-1.5</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>0.32082130082460703</v>
+        <v>1.7986209962091559E-2</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>0.10894749688090702</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.5325412426582235E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>-2</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>0.2689414213699951</v>
+        <v>6.6928509242848554E-3</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>9.8305966620740926E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.3296113341580309E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>-2.5</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>0.22270013882530884</v>
+        <v>2.4726231566347743E-3</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>8.6552393496248506E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.9330185827200961E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>-3</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>0.18242552380635635</v>
+        <v>9.1105119440064539E-4</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>7.4573226035166432E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.8204423602436531E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>-3.5</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>0.14804719803168948</v>
+        <v>3.3535013046647811E-4</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>6.3064612593327588E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6.7047534151294848E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>-4</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>0.11920292202211755</v>
+        <v>1.2339457598623172E-4</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>5.2496792701753253E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4675869952969781E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>-4.5</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>9.534946489910949E-2</v>
+        <v>4.5397868702434395E-5</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>4.3128972221281488E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9.0791615471903347E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>-5</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>7.5858180021243546E-2</v>
+        <v>1.6701421848095181E-5</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>3.5051858272554075E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.3402285821206868E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>-5.5</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>6.0086650174007626E-2</v>
+        <v>6.1441746022147182E-6</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>2.8238122322437029E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.2288273702666351E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>-6</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>4.7425873177566781E-2</v>
+        <v>2.2603242979035746E-6</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>2.2588329865456069E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.5206383776752853E-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>-6.5</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>3.7326887344129457E-2</v>
+        <v>8.3152802766413209E-7</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>1.7966795412664063E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.6630546724505427E-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>-7</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>2.9312230751356319E-2</v>
+        <v>3.0590222692562472E-7</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>1.422651193986778E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6.118042666989046E-7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>-7.5</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>2.2977369910025615E-2</v>
+        <v>1.1253516205509499E-7</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>1.1224705191021731E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.2507029878186457E-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>-8</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>1.7986209962091559E-2</v>
+        <v>4.1399375473943306E-8</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>8.8313531066455588E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8.2798747520070032E-8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>-8.5</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>1.4063627043245475E-2</v>
+        <v>1.5229979512760349E-8</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>6.9329207188169846E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0459958561616146E-8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>-9</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>1.098694263059318E-2</v>
+        <v>5.6027964061459406E-9</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>5.4331148611126171E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.1205592749509225E-8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>-9.5</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>8.5774854137119841E-3</v>
+        <v>2.0611536181902037E-9</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>4.2519560788447713E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.1223072278836992E-9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>-10</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>6.6928509242848554E-3</v>
+        <v>7.5825604221623851E-10</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>3.3240283353950773E-3</v>
+        <v>1.5165120832825725E-9</v>
       </c>
     </row>
   </sheetData>
@@ -1890,24 +1838,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>